<commit_message>
Print tensões em Volts + Simulações ANAFAS
</commit_message>
<xml_diff>
--- a/Parte 2/Scripts/Y0barra.xlsx
+++ b/Parte 2/Scripts/Y0barra.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ric\projects\Estudos\Trabalhos SEP\Parte 2\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3206637B-3011-4964-8D73-7F131FF29A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51396A5D-9676-447D-948B-B6B1F1082F58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Y0barra" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="33">
   <si>
     <t>1.14855-15.78475i</t>
   </si>
@@ -86,13 +86,46 @@
   </si>
   <si>
     <t>0.06521-0.24069i</t>
+  </si>
+  <si>
+    <t>Coluna 1</t>
+  </si>
+  <si>
+    <t>Coluna 2</t>
+  </si>
+  <si>
+    <t>Coluna 3</t>
+  </si>
+  <si>
+    <t>Coluna 4</t>
+  </si>
+  <si>
+    <t>Coluna 5</t>
+  </si>
+  <si>
+    <t>Coluna 6</t>
+  </si>
+  <si>
+    <t>Coluna 7</t>
+  </si>
+  <si>
+    <t>Coluna 8</t>
+  </si>
+  <si>
+    <t>Coluna 9</t>
+  </si>
+  <si>
+    <t>Coluna 10</t>
+  </si>
+  <si>
+    <t>Coluna 11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -223,6 +256,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -925,23 +964,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection sqref="A1:K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="3" max="3" width="20.5703125" customWidth="1"/>
     <col min="4" max="4" width="19.140625" customWidth="1"/>
     <col min="5" max="5" width="19.28515625" customWidth="1"/>
     <col min="6" max="6" width="20.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" customWidth="1"/>
+    <col min="8" max="8" width="19" customWidth="1"/>
     <col min="9" max="9" width="20.42578125" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="19" customWidth="1"/>
@@ -949,51 +988,51 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
-        <v>2</v>
+        <v>27</v>
       </c>
       <c r="G1" t="s">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>2</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s">
-        <v>2</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>2</v>
@@ -1005,7 +1044,7 @@
         <v>2</v>
       </c>
       <c r="H2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I2" t="s">
         <v>2</v>
@@ -1019,16 +1058,16 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E3" t="s">
         <v>2</v>
@@ -1057,13 +1096,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E4" t="s">
         <v>2</v>
@@ -1092,19 +1131,19 @@
         <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="G5" t="s">
         <v>2</v>
@@ -1113,7 +1152,7 @@
         <v>2</v>
       </c>
       <c r="I5" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J5" t="s">
         <v>2</v>
@@ -1136,19 +1175,19 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" t="s">
         <v>11</v>
       </c>
-      <c r="F6" t="s">
-        <v>13</v>
-      </c>
       <c r="G6" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="H6" t="s">
         <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="J6" t="s">
         <v>2</v>
@@ -1171,19 +1210,19 @@
         <v>2</v>
       </c>
       <c r="E7" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
         <v>14</v>
       </c>
-      <c r="G7" t="s">
-        <v>16</v>
-      </c>
       <c r="H7" t="s">
         <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
         <v>2</v>
@@ -1194,7 +1233,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -1209,13 +1248,13 @@
         <v>2</v>
       </c>
       <c r="F8" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="H8" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="I8" t="s">
         <v>2</v>
@@ -1229,7 +1268,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -1241,19 +1280,19 @@
         <v>2</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="F9" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="G9" t="s">
         <v>2</v>
       </c>
       <c r="H9" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="I9" t="s">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="J9" t="s">
         <v>2</v>
@@ -1276,10 +1315,10 @@
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="G10" t="s">
         <v>2</v>
@@ -1288,13 +1327,13 @@
         <v>2</v>
       </c>
       <c r="I10" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="J10" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="K10" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -1326,13 +1365,49 @@
         <v>2</v>
       </c>
       <c r="J11" t="s">
+        <v>19</v>
+      </c>
+      <c r="K11" t="s">
         <v>20</v>
       </c>
-      <c r="K11" t="s">
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" t="s">
+        <v>20</v>
+      </c>
+      <c r="K12" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>